<commit_message>
SCH - Header Pin 수정
</commit_message>
<xml_diff>
--- a/MCU PCB/1_Schematic/Plasma_LF_Gen_MCU_PL_V1.0_20180125.xlsx
+++ b/MCU PCB/1_Schematic/Plasma_LF_Gen_MCU_PL_V1.0_20180125.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
   <si>
     <t>No</t>
   </si>
@@ -309,25 +309,10 @@
     <t>HEADER_20X2</t>
   </si>
   <si>
-    <t>A1-40PA-2.54DSA</t>
-  </si>
-  <si>
-    <t>Hirose</t>
-  </si>
-  <si>
-    <t>2.54mm pitch 40-pin(20x2) Header</t>
-  </si>
-  <si>
     <t>J9,J10</t>
   </si>
   <si>
-    <t>14.3x4.05</t>
-  </si>
-  <si>
     <t>A1-10PA-2.54DSA</t>
-  </si>
-  <si>
-    <t>2.54mm pitch 10-pin(2x5) Header</t>
   </si>
   <si>
     <t>J103</t>
@@ -397,7 +382,74 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Hirose</t>
+    <t>FCI</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'nd Vendor</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>재고</t>
+  </si>
+  <si>
+    <t>ic114</t>
+  </si>
+  <si>
+    <t>YST-1502 SMD</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>영성정공</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.0x3.7</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5mm</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>TACH Switch 8.0x3.7, T=2.5mm SMD</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_LF_Generator MCU Board Part List</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>택배비</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>FCI</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>57102-G06-20LF</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>FCI</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>42x4.0</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5mm</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -405,54 +457,27 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>FCI</t>
+    <t>57102-G06-20LF</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>2'nd Vendor</t>
+    <t>2.00mm pitch 40-pin(20x2) Header Post=4mm Tail=2.5mm</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Unit Cost</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>재고</t>
-  </si>
-  <si>
-    <t>ic114</t>
-  </si>
-  <si>
-    <t>YST-1502 SMD</t>
+    <t>2.54mm pitch 10-pin(2x5) Header Post=5.84mm Tail=3.05mm</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>영성정공</t>
+    <t>12.7x4.83</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>8.0x3.7</t>
+    <t>54102-S08-10</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>2.5mm</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>TACH Switch 8.0x3.7, T=2.5mm SMD</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plasma_LF_Generator MCU Board Part List</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>택배비</t>
+    <t>5.84mm</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -460,9 +485,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -651,7 +675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,8 +867,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1153,19 +1183,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1309,30 +1326,30 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="34" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1">
@@ -1341,106 +1358,112 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="16" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="44" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="34" borderId="16" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="21" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="33" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="14" xfId="44" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="21" xfId="44" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="14" xfId="44" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1770,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U29"/>
+  <dimension ref="B1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1784,1221 +1807,1223 @@
     <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="67" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9" style="14"/>
+    <col min="8" max="9" width="9" style="13"/>
     <col min="10" max="10" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.375" style="10" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="26" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="N1" s="10"/>
-      <c r="P1" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="N1" s="9"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="J5" s="29" t="s">
+      <c r="H5" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="29" t="s">
+      <c r="L5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="N5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="O5" s="29" t="s">
+      <c r="M5" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="T5" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="P5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="R5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="U5" s="16"/>
+      <c r="U5" s="36"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
+      <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>7</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="19">
         <v>10</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="19">
         <f t="shared" ref="N6:N25" si="0">M6*G6</f>
         <v>70</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="17">
         <v>10</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="17">
         <f t="shared" ref="P6:P25" si="1">IF(G6&gt;O6,G6*M6,O6*M6)</f>
         <v>100</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="22"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="20"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>2</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>1</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25" t="s">
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="23">
         <v>10</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O7" s="26">
         <v>10</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="26">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q7" s="25" t="s">
+      <c r="Q7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="25" t="s">
+      <c r="R7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="27"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="23">
         <v>2</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="23">
         <v>10</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="26">
         <v>10</v>
       </c>
-      <c r="P8" s="28">
+      <c r="P8" s="26">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q8" s="25" t="s">
+      <c r="Q8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="25" t="s">
+      <c r="R8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="27"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="25"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <v>4</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="23">
         <v>2</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="25" t="s">
+      <c r="K9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="23">
         <v>10</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="O9" s="28">
+      <c r="O9" s="26">
         <v>10</v>
       </c>
-      <c r="P9" s="28">
+      <c r="P9" s="26">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q9" s="25" t="s">
+      <c r="Q9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="27"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="25"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <v>5</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="23">
         <v>2</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25" t="s">
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="23">
         <v>210</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="23">
         <f t="shared" si="0"/>
         <v>420</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="26">
         <v>25</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="26">
         <f t="shared" si="1"/>
         <v>5250</v>
       </c>
-      <c r="Q10" s="25" t="s">
+      <c r="Q10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="25" t="s">
+      <c r="R10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="27"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="25"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>6</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="23">
         <v>1</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25" t="s">
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="23">
         <v>10</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O11" s="28">
+      <c r="O11" s="26">
         <v>100</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11" s="26">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="Q11" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="27"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="25"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <v>7</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="24">
         <v>470</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="23">
         <v>5</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25" t="s">
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="23">
         <v>10</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="23">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O12" s="28">
+      <c r="O12" s="26">
         <v>100</v>
       </c>
-      <c r="P12" s="28">
+      <c r="P12" s="26">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Q12" s="25" t="s">
+      <c r="Q12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="R12" s="25" t="s">
+      <c r="R12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="27"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="25"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <v>8</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="23">
         <v>7</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25" t="s">
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="25" t="s">
+      <c r="K13" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="23">
         <v>10</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="23">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="O13" s="28">
+      <c r="O13" s="26">
         <v>100</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="26">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Q13" s="25" t="s">
+      <c r="Q13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="25" t="s">
+      <c r="R13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="27"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="25"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>9</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="24">
         <v>0</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="23">
         <v>5</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25" t="s">
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="K14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="23">
         <v>10</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="23">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O14" s="28">
+      <c r="O14" s="26">
         <v>100</v>
       </c>
-      <c r="P14" s="28">
+      <c r="P14" s="26">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Q14" s="25" t="s">
+      <c r="Q14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="R14" s="25" t="s">
+      <c r="R14" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="27"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="25"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <v>10</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="23">
         <v>5</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="K15" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="23">
         <v>20</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="23">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28">
+      <c r="O15" s="26"/>
+      <c r="P15" s="26">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q15" s="25" t="s">
+      <c r="Q15" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="27"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="25"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <v>11</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="23">
         <v>1</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25" t="s">
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="K16" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="23">
         <v>480</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="23">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="26">
         <v>1</v>
       </c>
-      <c r="P16" s="28">
+      <c r="P16" s="26">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="Q16" s="25" t="s">
+      <c r="Q16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="R16" s="25" t="s">
+      <c r="R16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="S16" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="T16" s="25"/>
-      <c r="U16" s="27"/>
+      <c r="S16" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="T16" s="23"/>
+      <c r="U16" s="25"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>12</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="23">
         <v>4</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="K17" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="23">
         <v>180</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="23">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="O17" s="28">
+      <c r="O17" s="26">
         <v>1</v>
       </c>
-      <c r="P17" s="28">
+      <c r="P17" s="26">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="Q17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="R17" s="25" t="s">
+      <c r="R17" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="S17" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="T17" s="25"/>
-      <c r="U17" s="27"/>
+      <c r="S17" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="T17" s="23"/>
+      <c r="U17" s="25"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>13</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="23">
         <v>1</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25" t="s">
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="K18" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="L18" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="23">
         <v>3970</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="23">
         <f t="shared" si="0"/>
         <v>3970</v>
       </c>
-      <c r="O18" s="28">
+      <c r="O18" s="26">
         <v>1</v>
       </c>
-      <c r="P18" s="28">
+      <c r="P18" s="26">
         <f t="shared" si="1"/>
         <v>3970</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="Q18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="R18" s="25" t="s">
+      <c r="R18" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="S18" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="T18" s="25"/>
-      <c r="U18" s="27"/>
+      <c r="S18" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="T18" s="23"/>
+      <c r="U18" s="25"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>14</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="23">
         <v>1</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25" t="s">
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="K19" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="23">
         <v>1750</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="23">
         <f t="shared" si="0"/>
         <v>1750</v>
       </c>
-      <c r="O19" s="28">
+      <c r="O19" s="26">
         <v>1</v>
       </c>
-      <c r="P19" s="28">
+      <c r="P19" s="26">
         <f t="shared" si="1"/>
         <v>1750</v>
       </c>
-      <c r="Q19" s="25" t="s">
+      <c r="Q19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="25" t="s">
+      <c r="R19" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="S19" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="T19" s="25"/>
-      <c r="U19" s="27"/>
+      <c r="S19" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="T19" s="23"/>
+      <c r="U19" s="25"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>15</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="23">
         <v>1</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25" t="s">
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="25" t="s">
+      <c r="K20" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="L20" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="23">
         <v>120</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="23">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="O20" s="32">
+      <c r="O20" s="29">
         <v>20</v>
       </c>
-      <c r="P20" s="28">
+      <c r="P20" s="26">
         <f t="shared" si="1"/>
         <v>2400</v>
       </c>
-      <c r="Q20" s="25" t="s">
+      <c r="Q20" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="R20" s="25" t="s">
+      <c r="R20" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="S20" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="T20" s="25"/>
-      <c r="U20" s="27"/>
+      <c r="S20" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="T20" s="23"/>
+      <c r="U20" s="25"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
+      <c r="B21" s="16">
         <v>16</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="23">
+        <v>2</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="25">
-        <v>2</v>
-      </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" s="25">
-        <v>1.2</v>
-      </c>
-      <c r="M21" s="25">
-        <v>1500</v>
-      </c>
-      <c r="N21" s="25">
+      <c r="K21" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="M21" s="23">
+        <v>4290</v>
+      </c>
+      <c r="N21" s="23">
         <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="O21" s="25">
-        <v>122</v>
-      </c>
-      <c r="P21" s="28">
+        <v>8580</v>
+      </c>
+      <c r="O21" s="23">
+        <v>1</v>
+      </c>
+      <c r="P21" s="26">
         <f t="shared" si="1"/>
-        <v>183000</v>
-      </c>
-      <c r="Q21" s="25" t="s">
+        <v>8580</v>
+      </c>
+      <c r="Q21" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="R21" s="25" t="s">
+      <c r="R21" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="S21" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="T21" s="25"/>
-      <c r="U21" s="27"/>
+      <c r="S21" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="T21" s="23"/>
+      <c r="U21" s="25"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <v>17</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="25">
+      <c r="C22" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="23">
         <v>1</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="K22" s="25">
-        <v>0</v>
-      </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25">
-        <v>740</v>
-      </c>
-      <c r="N22" s="25">
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="M22" s="23">
+        <v>880</v>
+      </c>
+      <c r="N22" s="23">
         <f t="shared" si="0"/>
-        <v>740</v>
-      </c>
-      <c r="O22" s="25">
+        <v>880</v>
+      </c>
+      <c r="O22" s="23">
         <v>1</v>
       </c>
-      <c r="P22" s="28">
+      <c r="P22" s="26">
         <f t="shared" si="1"/>
-        <v>740</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="R22" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="S22" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="T22" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="U22" s="27" t="s">
-        <v>126</v>
+        <v>880</v>
+      </c>
+      <c r="Q22" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="R22" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="S22" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="U22" s="25" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <v>18</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="25">
+      <c r="C23" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="23">
         <v>1</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="M23" s="25">
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="M23" s="23">
         <v>100</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="23">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="29">
         <v>10</v>
       </c>
-      <c r="P23" s="28">
+      <c r="P23" s="26">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="Q23" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="R23" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="S23" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="T23" s="25"/>
-      <c r="U23" s="27"/>
+      <c r="Q23" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="S23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="T23" s="23"/>
+      <c r="U23" s="25"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="18">
+      <c r="B24" s="16">
         <v>19</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="25">
-        <v>1</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="L24" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="M24" s="25">
+      <c r="L24" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M24" s="23">
         <v>1750</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="23">
         <f t="shared" si="0"/>
         <v>1750</v>
       </c>
-      <c r="O24" s="25">
+      <c r="O24" s="23">
         <v>5</v>
       </c>
-      <c r="P24" s="28">
+      <c r="P24" s="26">
         <f t="shared" si="1"/>
         <v>8750</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="R24" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="S24" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="T24" s="25"/>
-      <c r="U24" s="27"/>
+      <c r="Q24" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="R24" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="S24" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="T24" s="23"/>
+      <c r="U24" s="25"/>
     </row>
     <row r="25" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="38">
         <v>20</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="34">
+        <v>1</v>
+      </c>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="K25" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="37">
-        <v>1</v>
-      </c>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="K25" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="L25" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="M25" s="37">
+      <c r="L25" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="M25" s="34">
         <v>880</v>
       </c>
-      <c r="N25" s="37">
+      <c r="N25" s="34">
         <f t="shared" si="0"/>
         <v>880</v>
       </c>
-      <c r="O25" s="37">
+      <c r="O25" s="34">
         <v>1000</v>
       </c>
-      <c r="P25" s="31">
+      <c r="P25" s="28">
         <f t="shared" si="1"/>
         <v>880000</v>
       </c>
-      <c r="Q25" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="R25" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="S25" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="T25" s="37"/>
+      <c r="Q25" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="R25" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S25" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="T25" s="34"/>
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="34">
+      <c r="B26" s="31">
         <v>21</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="32">
         <v>3</v>
       </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35" t="s">
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="K26" s="35" t="s">
+      <c r="K26" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="L26" s="35" t="s">
+      <c r="L26" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35">
+      <c r="M26" s="32"/>
+      <c r="N26" s="32">
         <f>M26*G26</f>
         <v>0</v>
       </c>
@@ -3009,15 +3034,15 @@
         <f>IF(G26&gt;O26,G26*M26,O26*M26)</f>
         <v>0</v>
       </c>
-      <c r="Q26" s="35" t="s">
+      <c r="Q26" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="R26" s="35" t="s">
+      <c r="R26" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="36"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="33"/>
     </row>
     <row r="27" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
@@ -3054,10 +3079,10 @@
         <f>M27*G27</f>
         <v>0</v>
       </c>
-      <c r="O27" s="8">
+      <c r="O27" s="7">
         <v>100</v>
       </c>
-      <c r="P27" s="8">
+      <c r="P27" s="7">
         <f>IF(G27&gt;O27,G27*M27,O27*M27)</f>
         <v>0</v>
       </c>
@@ -3071,31 +3096,34 @@
       <c r="T27" s="6"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="2:21" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="N28" s="17">
+    <row r="28" spans="2:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="N28" s="15">
         <f>SUM(N6:N25)</f>
-        <v>14330</v>
-      </c>
-      <c r="P28" s="17">
+        <v>20050</v>
+      </c>
+      <c r="P28" s="15">
         <f>SUM(P6:P25)</f>
-        <v>1092560</v>
+        <v>918280</v>
       </c>
     </row>
     <row r="29" spans="2:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+        <v>114</v>
+      </c>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
       <c r="M29" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N29" s="17">
+        <v>132</v>
+      </c>
+      <c r="N29" s="15">
         <v>5000</v>
       </c>
-      <c r="P29" s="12"/>
+      <c r="P29" s="11"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="E32" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="B5:L5"/>

</xml_diff>